<commit_message>
Previo a entrega minuta 29-ago
</commit_message>
<xml_diff>
--- a/Minuta_PetsHeroe.xlsx
+++ b/Minuta_PetsHeroe.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryangutierrez/Documents/Dotech/PetsHeroe/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8AB9C8-AB5F-E24D-BD61-45ABA55C5595}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="7">
   <si>
     <t>Ok</t>
   </si>
@@ -32,16 +33,10 @@
     <t>OK</t>
   </si>
   <si>
-    <t>Pendiente agregar tipo_asociado en la respuesta del ws</t>
-  </si>
-  <si>
     <t>Pendiente en iOS</t>
   </si>
   <si>
     <t>Pendiente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pendiente codigos validos para mascotas </t>
   </si>
   <si>
     <t>Pendiente ¿A que se refiere?</t>
@@ -56,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -104,6 +99,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -371,11 +369,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -385,10 +383,10 @@
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
@@ -412,7 +410,7 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
@@ -428,7 +426,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
@@ -444,7 +442,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
@@ -460,7 +458,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.2">
@@ -468,7 +466,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.2">
@@ -492,7 +490,7 @@
         <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.2">
@@ -500,7 +498,7 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.2">
@@ -524,7 +522,7 @@
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.2">
@@ -532,7 +530,7 @@
         <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.2">
@@ -540,7 +538,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.2">
@@ -556,7 +554,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>